<commit_message>
Update a sample project file and Excel files.
</commit_message>
<xml_diff>
--- a/Japanese/プロジェクトサンプル/変則2交代学習/source/4月ランダム予定.xlsx
+++ b/Japanese/プロジェクトサンプル/変則2交代学習/source/4月ランダム予定.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="53" count="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="58" count="348">
   <si>
     <t>スタッフ名</t>
   </si>
@@ -40,7 +40,7 @@
     <t>第5週</t>
   </si>
   <si>
-    <t>チーム</t>
+    <t>コメント</t>
   </si>
   <si>
     <t>木</t>
@@ -64,16 +64,16 @@
     <t>水</t>
   </si>
   <si>
-    <t>川畑　拓也</t>
+    <t>スタッフ1</t>
   </si>
   <si>
     <t>週</t>
   </si>
   <si>
-    <t>中田　拓実</t>
-  </si>
-  <si>
-    <t>A</t>
+    <t>スタッフ2</t>
+  </si>
+  <si>
+    <t>夜勤4回まで</t>
   </si>
   <si>
     <t>★</t>
@@ -88,91 +88,106 @@
     <t>長</t>
   </si>
   <si>
-    <t>高橋　真央</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>友安　美琴</t>
-  </si>
-  <si>
-    <t>降矢　悠司</t>
-  </si>
-  <si>
-    <t>横山　加奈</t>
-  </si>
-  <si>
-    <t>渡邊　夏希</t>
-  </si>
-  <si>
-    <t>髙田　実歩</t>
-  </si>
-  <si>
-    <t>藤本　春佳</t>
-  </si>
-  <si>
-    <t>永田　慎治</t>
-  </si>
-  <si>
-    <t>花房　秀明</t>
-  </si>
-  <si>
-    <t>山田　伸明</t>
-  </si>
-  <si>
-    <t>山上　恵実</t>
-  </si>
-  <si>
-    <t>徳重　駿介</t>
-  </si>
-  <si>
-    <t>水越　智哉</t>
-  </si>
-  <si>
-    <t>杉村　青空</t>
-  </si>
-  <si>
-    <t>長坂　有里子</t>
-  </si>
-  <si>
-    <t>藤本　望</t>
-  </si>
-  <si>
-    <t>安達　由佳</t>
-  </si>
-  <si>
-    <t>西尾　貴宏</t>
-  </si>
-  <si>
-    <t>木口　瞳子</t>
-  </si>
-  <si>
-    <t>上道　啓太</t>
-  </si>
-  <si>
-    <t>松田　瑠美</t>
-  </si>
-  <si>
-    <t>水野　真吾</t>
-  </si>
-  <si>
-    <t>石嶺　利樹</t>
-  </si>
-  <si>
-    <t>末堂　厚</t>
-  </si>
-  <si>
-    <t>加藤　清澄</t>
-  </si>
-  <si>
-    <t>鎬昂　昇</t>
-  </si>
-  <si>
-    <t>本部　以蔵</t>
-  </si>
-  <si>
-    <t>松本　梢江</t>
+    <t>スタッフ3</t>
+  </si>
+  <si>
+    <t>スタッフ4</t>
+  </si>
+  <si>
+    <t>スタッフ5</t>
+  </si>
+  <si>
+    <t>スタッフ6</t>
+  </si>
+  <si>
+    <t>スタッフ7</t>
+  </si>
+  <si>
+    <t>スタッフ8</t>
+  </si>
+  <si>
+    <t>スタッフ9</t>
+  </si>
+  <si>
+    <t>夜勤3回まで</t>
+  </si>
+  <si>
+    <t>スタッフ10</t>
+  </si>
+  <si>
+    <t>スタッフ11</t>
+  </si>
+  <si>
+    <t>スタッフ12</t>
+  </si>
+  <si>
+    <t>スタッフ13</t>
+  </si>
+  <si>
+    <t>スタッフ14</t>
+  </si>
+  <si>
+    <t>スタッフ15</t>
+  </si>
+  <si>
+    <t>スタッフ16</t>
+  </si>
+  <si>
+    <t>新人　月前半長夜勤なし　</t>
+  </si>
+  <si>
+    <t>スタッフ17</t>
+  </si>
+  <si>
+    <t>スタッフ18</t>
+  </si>
+  <si>
+    <t>スタッフ19</t>
+  </si>
+  <si>
+    <t>スタッフ20</t>
+  </si>
+  <si>
+    <t>土日休み日勤のみ</t>
+  </si>
+  <si>
+    <t>スタッフ21</t>
+  </si>
+  <si>
+    <t>夜勤土日のみ3回まで</t>
+  </si>
+  <si>
+    <t>スタッフ22</t>
+  </si>
+  <si>
+    <t>長入明　水木金3回まで</t>
+  </si>
+  <si>
+    <t>スタッフ23</t>
+  </si>
+  <si>
+    <t>スタッフ24</t>
+  </si>
+  <si>
+    <t>スタッフ25</t>
+  </si>
+  <si>
+    <t>スタッフ26</t>
+  </si>
+  <si>
+    <t>スタッフ27</t>
+  </si>
+  <si>
+    <t>スタッフ28</t>
+  </si>
+  <si>
+    <t>スタッフ29</t>
+  </si>
+  <si>
+    <t>スタッフ30</t>
+  </si>
+  <si>
+    <t>新人　月前半長夜勤なし</t>
   </si>
 </sst>
 </file>
@@ -740,19 +755,19 @@
         <v>16</v>
       </c>
       <c r="B4" s="15"/>
-      <c r="C4" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="14" t="s">
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H4" s="14" t="s">
@@ -853,19 +868,19 @@
       <c r="B5" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="14" t="s">
+      <c r="E5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H5" s="14" t="s">
@@ -910,21 +925,21 @@
         <v>24</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H6" s="1"/>
@@ -966,24 +981,22 @@
     </row>
     <row r="7" spans="1:37">
       <c r="A7" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="15"/>
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H7" s="1"/>
@@ -1025,24 +1038,22 @@
     </row>
     <row r="8" spans="1:37">
       <c r="A8" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="15"/>
+      <c r="C8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H8" s="1"/>
@@ -1084,24 +1095,22 @@
     </row>
     <row r="9" spans="1:37">
       <c r="A9" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="15"/>
+      <c r="C9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="1" t="s">
         <v>20</v>
       </c>
       <c r="H9" s="1"/>
@@ -1145,24 +1154,22 @@
     </row>
     <row r="10" spans="1:37">
       <c r="A10" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="15"/>
+      <c r="C10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="14" t="s">
+      <c r="F10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H10" s="1"/>
@@ -1204,24 +1211,22 @@
     </row>
     <row r="11" spans="1:37">
       <c r="A11" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="15"/>
+      <c r="C11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H11" s="1"/>
@@ -1263,24 +1268,24 @@
     </row>
     <row r="12" spans="1:37">
       <c r="A12" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="14" t="s">
+      <c r="F12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H12" s="1"/>
@@ -1322,22 +1327,20 @@
       <c r="A13" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="14" t="s">
+      <c r="B13" s="15"/>
+      <c r="C13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="14" t="s">
+      <c r="E13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H13" s="1"/>
@@ -1381,22 +1384,20 @@
       <c r="A14" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="14" t="s">
+      <c r="B14" s="15"/>
+      <c r="C14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="14" t="s">
+      <c r="D14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G14" s="14" t="s">
+      <c r="F14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H14" s="1"/>
@@ -1438,22 +1439,20 @@
       <c r="A15" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" s="14" t="s">
+      <c r="B15" s="15"/>
+      <c r="C15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G15" s="14" t="s">
+      <c r="G15" s="1" t="s">
         <v>20</v>
       </c>
       <c r="H15" s="1"/>
@@ -1497,22 +1496,20 @@
       <c r="A16" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="14" t="s">
+      <c r="B16" s="15"/>
+      <c r="C16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G16" s="14" t="s">
+      <c r="E16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H16" s="1"/>
@@ -1556,22 +1553,20 @@
       <c r="A17" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="14" t="s">
+      <c r="B17" s="15"/>
+      <c r="C17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="F17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G17" s="14" t="s">
+      <c r="G17" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H17" s="1"/>
@@ -1615,22 +1610,20 @@
       <c r="A18" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="G18" s="14" t="s">
+      <c r="B18" s="15"/>
+      <c r="C18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H18" s="1"/>
@@ -1675,21 +1668,21 @@
         <v>38</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="14" t="s">
+      <c r="E19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="F19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G19" s="14" t="s">
+      <c r="G19" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H19" s="1"/>
@@ -1731,24 +1724,22 @@
     </row>
     <row r="20" spans="1:37">
       <c r="A20" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="15"/>
+      <c r="C20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H20" s="1"/>
@@ -1790,24 +1781,22 @@
     </row>
     <row r="21" spans="1:37">
       <c r="A21" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="15"/>
+      <c r="C21" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="14" t="s">
+      <c r="E21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G21" s="14" t="s">
+      <c r="F21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H21" s="1"/>
@@ -1849,24 +1838,22 @@
     </row>
     <row r="22" spans="1:37">
       <c r="A22" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="15"/>
+      <c r="C22" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="14" t="s">
+      <c r="D22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E22" s="14" t="s">
+      <c r="E22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F22" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G22" s="14" t="s">
+      <c r="F22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H22" s="1"/>
@@ -1908,24 +1895,24 @@
     </row>
     <row r="23" spans="1:37">
       <c r="A23" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="D23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E23" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G23" s="14" t="s">
+      <c r="E23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H23" s="1"/>
@@ -1967,24 +1954,24 @@
     </row>
     <row r="24" spans="1:37">
       <c r="A24" s="8" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F24" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G24" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H24" s="1"/>
@@ -2026,24 +2013,24 @@
     </row>
     <row r="25" spans="1:37">
       <c r="A25" s="8" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F25" s="14" t="s">
+      <c r="F25" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G25" s="14" t="s">
+      <c r="G25" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H25" s="1"/>
@@ -2083,24 +2070,22 @@
     </row>
     <row r="26" spans="1:37">
       <c r="A26" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E26" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="F26" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="G26" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="15"/>
+      <c r="C26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H26" s="1"/>
@@ -2142,24 +2127,22 @@
     </row>
     <row r="27" spans="1:37">
       <c r="A27" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="15"/>
+      <c r="C27" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F27" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G27" s="14" t="s">
+      <c r="E27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H27" s="14" t="s">
@@ -2201,24 +2184,22 @@
     </row>
     <row r="28" spans="1:37">
       <c r="A28" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D28" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E28" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F28" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G28" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="15"/>
+      <c r="C28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H28" s="1"/>
@@ -2264,24 +2245,22 @@
     </row>
     <row r="29" spans="1:37">
       <c r="A29" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C29" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" s="15"/>
+      <c r="C29" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="D29" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E29" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F29" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G29" s="14" t="s">
+      <c r="E29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H29" s="1"/>
@@ -2323,24 +2302,22 @@
     </row>
     <row r="30" spans="1:37">
       <c r="A30" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C30" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D30" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F30" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="15"/>
+      <c r="C30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G30" s="14" t="s">
+      <c r="G30" s="1" t="s">
         <v>20</v>
       </c>
       <c r="H30" s="1"/>
@@ -2382,24 +2359,22 @@
     </row>
     <row r="31" spans="1:37">
       <c r="A31" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C31" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D31" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E31" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31" s="15"/>
+      <c r="C31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F31" s="14" t="s">
+      <c r="F31" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G31" s="14" t="s">
+      <c r="G31" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H31" s="1"/>
@@ -2439,24 +2414,22 @@
     </row>
     <row r="32" spans="1:37">
       <c r="A32" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C32" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E32" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F32" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" s="15"/>
+      <c r="C32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G32" s="14" t="s">
+      <c r="G32" s="1" t="s">
         <v>20</v>
       </c>
       <c r="H32" s="1"/>
@@ -2498,24 +2471,24 @@
     </row>
     <row r="33" spans="1:37">
       <c r="A33" s="4" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C33" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D33" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E33" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F33" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="G33" s="14" t="s">
+      <c r="D33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H33" s="1"/>

</xml_diff>

<commit_message>
Update a sample project and excel files
</commit_message>
<xml_diff>
--- a/Japanese/プロジェクトサンプル/変則2交代学習/source/4月ランダム予定.xlsx
+++ b/Japanese/プロジェクトサンプル/変則2交代学習/source/4月ランダム予定.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="58" count="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="60" count="353">
   <si>
     <t>スタッフ名</t>
   </si>
@@ -97,9 +97,15 @@
     <t>スタッフ5</t>
   </si>
   <si>
+    <t>委1</t>
+  </si>
+  <si>
     <t>スタッフ6</t>
   </si>
   <si>
+    <t>委2</t>
+  </si>
+  <si>
     <t>スタッフ7</t>
   </si>
   <si>
@@ -148,22 +154,22 @@
     <t>スタッフ20</t>
   </si>
   <si>
+    <t>スタッフ21</t>
+  </si>
+  <si>
+    <t>夜勤土日のみ3回まで</t>
+  </si>
+  <si>
+    <t>スタッフ22</t>
+  </si>
+  <si>
+    <t>長入明　水木金3回まで</t>
+  </si>
+  <si>
+    <t>スタッフ23</t>
+  </si>
+  <si>
     <t>土日休み日勤のみ</t>
-  </si>
-  <si>
-    <t>スタッフ21</t>
-  </si>
-  <si>
-    <t>夜勤土日のみ3回まで</t>
-  </si>
-  <si>
-    <t>スタッフ22</t>
-  </si>
-  <si>
-    <t>長入明　水木金3回まで</t>
-  </si>
-  <si>
-    <t>スタッフ23</t>
   </si>
   <si>
     <t>スタッフ24</t>
@@ -227,7 +233,7 @@
       <charset val="0"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none">
         <fgColor indexed="64"/>
@@ -267,6 +273,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="26"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -365,7 +377,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="41">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyFill="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyFill="0" applyProtection="0"/>
@@ -434,6 +446,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyAlignment="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -492,39 +507,39 @@
       <c r="H1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
       <c r="O1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
       <c r="V1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="W1" s="16"/>
-      <c r="X1" s="16"/>
-      <c r="Y1" s="16"/>
-      <c r="Z1" s="16"/>
-      <c r="AA1" s="16"/>
-      <c r="AB1" s="16"/>
+      <c r="W1" s="17"/>
+      <c r="X1" s="17"/>
+      <c r="Y1" s="17"/>
+      <c r="Z1" s="17"/>
+      <c r="AA1" s="17"/>
+      <c r="AB1" s="17"/>
       <c r="AC1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="AD1" s="16"/>
-      <c r="AE1" s="16"/>
-      <c r="AF1" s="16"/>
-      <c r="AG1" s="16"/>
-      <c r="AH1" s="16"/>
-      <c r="AI1" s="20"/>
+      <c r="AD1" s="17"/>
+      <c r="AE1" s="17"/>
+      <c r="AF1" s="17"/>
+      <c r="AG1" s="17"/>
+      <c r="AH1" s="17"/>
+      <c r="AI1" s="21"/>
       <c r="AJ1" s="2" t="s">
         <v>7</v>
       </c>
@@ -550,88 +565,88 @@
       <c r="G2" s="8">
         <v>31</v>
       </c>
-      <c r="H2" s="17">
+      <c r="H2" s="18">
         <v>1</v>
       </c>
-      <c r="I2" s="17">
+      <c r="I2" s="18">
         <v>2</v>
       </c>
-      <c r="J2" s="17">
+      <c r="J2" s="18">
         <v>3</v>
       </c>
-      <c r="K2" s="17">
+      <c r="K2" s="18">
         <v>4</v>
       </c>
-      <c r="L2" s="18">
+      <c r="L2" s="19">
         <v>5</v>
       </c>
-      <c r="M2" s="19">
+      <c r="M2" s="20">
         <v>6</v>
       </c>
-      <c r="N2" s="17">
+      <c r="N2" s="18">
         <v>7</v>
       </c>
-      <c r="O2" s="17">
+      <c r="O2" s="18">
         <v>8</v>
       </c>
-      <c r="P2" s="17">
+      <c r="P2" s="18">
         <v>9</v>
       </c>
-      <c r="Q2" s="17">
+      <c r="Q2" s="18">
         <v>10</v>
       </c>
-      <c r="R2" s="17">
+      <c r="R2" s="18">
         <v>11</v>
       </c>
-      <c r="S2" s="18">
-        <v>12</v>
-      </c>
-      <c r="T2" s="19">
+      <c r="S2" s="19">
+        <v>12</v>
+      </c>
+      <c r="T2" s="20">
         <v>13</v>
       </c>
-      <c r="U2" s="17">
+      <c r="U2" s="18">
         <v>14</v>
       </c>
-      <c r="V2" s="17">
+      <c r="V2" s="18">
         <v>15</v>
       </c>
-      <c r="W2" s="17">
+      <c r="W2" s="18">
         <v>16</v>
       </c>
-      <c r="X2" s="17">
-        <v>17</v>
-      </c>
-      <c r="Y2" s="17">
+      <c r="X2" s="18">
+        <v>17</v>
+      </c>
+      <c r="Y2" s="18">
         <v>18</v>
       </c>
-      <c r="Z2" s="18">
+      <c r="Z2" s="19">
         <v>19</v>
       </c>
-      <c r="AA2" s="19">
+      <c r="AA2" s="20">
         <v>20</v>
       </c>
-      <c r="AB2" s="17">
+      <c r="AB2" s="18">
         <v>21</v>
       </c>
-      <c r="AC2" s="17">
+      <c r="AC2" s="18">
         <v>22</v>
       </c>
-      <c r="AD2" s="17">
+      <c r="AD2" s="18">
         <v>23</v>
       </c>
-      <c r="AE2" s="17">
+      <c r="AE2" s="18">
         <v>24</v>
       </c>
-      <c r="AF2" s="17">
+      <c r="AF2" s="18">
         <v>25</v>
       </c>
-      <c r="AG2" s="18">
+      <c r="AG2" s="19">
         <v>26</v>
       </c>
-      <c r="AH2" s="19">
+      <c r="AH2" s="20">
         <v>27</v>
       </c>
-      <c r="AI2" s="17">
+      <c r="AI2" s="18">
         <v>28</v>
       </c>
       <c r="AJ2" s="11">
@@ -1040,7 +1055,9 @@
       <c r="A8" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="15"/>
+      <c r="B8" s="15" t="s">
+        <v>27</v>
+      </c>
       <c r="C8" s="1" t="s">
         <v>12</v>
       </c>
@@ -1095,9 +1112,11 @@
     </row>
     <row r="9" spans="1:37">
       <c r="A9" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="15"/>
+        <v>28</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>29</v>
+      </c>
       <c r="C9" s="1" t="s">
         <v>12</v>
       </c>
@@ -1154,7 +1173,7 @@
     </row>
     <row r="10" spans="1:37">
       <c r="A10" s="8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B10" s="15"/>
       <c r="C10" s="1" t="s">
@@ -1211,7 +1230,7 @@
     </row>
     <row r="11" spans="1:37">
       <c r="A11" s="8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B11" s="15"/>
       <c r="C11" s="1" t="s">
@@ -1268,10 +1287,10 @@
     </row>
     <row r="12" spans="1:37">
       <c r="A12" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>23</v>
@@ -1325,7 +1344,7 @@
     </row>
     <row r="13" spans="1:37">
       <c r="A13" s="8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B13" s="15"/>
       <c r="C13" s="1" t="s">
@@ -1382,7 +1401,7 @@
     </row>
     <row r="14" spans="1:37">
       <c r="A14" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="1" t="s">
@@ -1437,9 +1456,11 @@
     </row>
     <row r="15" spans="1:37">
       <c r="A15" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="15"/>
+        <v>36</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>29</v>
+      </c>
       <c r="C15" s="1" t="s">
         <v>17</v>
       </c>
@@ -1494,7 +1515,7 @@
     </row>
     <row r="16" spans="1:37">
       <c r="A16" s="8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B16" s="15"/>
       <c r="C16" s="1" t="s">
@@ -1551,7 +1572,7 @@
     </row>
     <row r="17" spans="1:37">
       <c r="A17" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B17" s="15"/>
       <c r="C17" s="1" t="s">
@@ -1608,7 +1629,7 @@
     </row>
     <row r="18" spans="1:37">
       <c r="A18" s="8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B18" s="15"/>
       <c r="C18" s="1" t="s">
@@ -1665,10 +1686,10 @@
     </row>
     <row r="19" spans="1:37">
       <c r="A19" s="8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>12</v>
@@ -1724,7 +1745,7 @@
     </row>
     <row r="20" spans="1:37">
       <c r="A20" s="8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B20" s="15"/>
       <c r="C20" s="1" t="s">
@@ -1781,7 +1802,7 @@
     </row>
     <row r="21" spans="1:37">
       <c r="A21" s="8" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B21" s="15"/>
       <c r="C21" s="1" t="s">
@@ -1838,7 +1859,7 @@
     </row>
     <row r="22" spans="1:37">
       <c r="A22" s="8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B22" s="15"/>
       <c r="C22" s="1" t="s">
@@ -1895,12 +1916,10 @@
     </row>
     <row r="23" spans="1:37">
       <c r="A23" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="15"/>
+      <c r="C23" s="16" t="s">
         <v>21</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -1954,10 +1973,10 @@
     </row>
     <row r="24" spans="1:37">
       <c r="A24" s="8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>12</v>
@@ -2013,10 +2032,10 @@
     </row>
     <row r="25" spans="1:37">
       <c r="A25" s="8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>12</v>
@@ -2070,9 +2089,11 @@
     </row>
     <row r="26" spans="1:37">
       <c r="A26" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B26" s="15"/>
+        <v>50</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>51</v>
+      </c>
       <c r="C26" s="1" t="s">
         <v>17</v>
       </c>
@@ -2127,7 +2148,7 @@
     </row>
     <row r="27" spans="1:37">
       <c r="A27" s="8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B27" s="15"/>
       <c r="C27" s="1" t="s">
@@ -2184,7 +2205,7 @@
     </row>
     <row r="28" spans="1:37">
       <c r="A28" s="8" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B28" s="15"/>
       <c r="C28" s="1" t="s">
@@ -2245,9 +2266,11 @@
     </row>
     <row r="29" spans="1:37">
       <c r="A29" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="B29" s="15"/>
+        <v>54</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>27</v>
+      </c>
       <c r="C29" s="1" t="s">
         <v>20</v>
       </c>
@@ -2302,9 +2325,11 @@
     </row>
     <row r="30" spans="1:37">
       <c r="A30" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B30" s="15"/>
+        <v>55</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>29</v>
+      </c>
       <c r="C30" s="1" t="s">
         <v>12</v>
       </c>
@@ -2359,7 +2384,7 @@
     </row>
     <row r="31" spans="1:37">
       <c r="A31" s="8" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B31" s="15"/>
       <c r="C31" s="1" t="s">
@@ -2414,7 +2439,7 @@
     </row>
     <row r="32" spans="1:37">
       <c r="A32" s="8" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B32" s="15"/>
       <c r="C32" s="1" t="s">
@@ -2471,10 +2496,10 @@
     </row>
     <row r="33" spans="1:37">
       <c r="A33" s="4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Add a sample project for ICU committee.
</commit_message>
<xml_diff>
--- a/Japanese/プロジェクトサンプル/変則2交代学習/source/4月ランダム予定.xlsx
+++ b/Japanese/プロジェクトサンプル/変則2交代学習/source/4月ランダム予定.xlsx
@@ -169,13 +169,13 @@
     <t>スタッフ23</t>
   </si>
   <si>
+    <t>スタッフ24</t>
+  </si>
+  <si>
+    <t>スタッフ25</t>
+  </si>
+  <si>
     <t>土日休み日勤のみ</t>
-  </si>
-  <si>
-    <t>スタッフ24</t>
-  </si>
-  <si>
-    <t>スタッフ25</t>
   </si>
   <si>
     <t>スタッフ26</t>
@@ -233,7 +233,7 @@
       <charset val="0"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none">
         <fgColor indexed="64"/>
@@ -273,12 +273,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="26"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -377,7 +371,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyFill="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyFill="0" applyProtection="0"/>
@@ -446,9 +440,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyAlignment="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -507,39 +498,39 @@
       <c r="H1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
       <c r="O1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="17"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
       <c r="V1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="W1" s="17"/>
-      <c r="X1" s="17"/>
-      <c r="Y1" s="17"/>
-      <c r="Z1" s="17"/>
-      <c r="AA1" s="17"/>
-      <c r="AB1" s="17"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="16"/>
+      <c r="AA1" s="16"/>
+      <c r="AB1" s="16"/>
       <c r="AC1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="AD1" s="17"/>
-      <c r="AE1" s="17"/>
-      <c r="AF1" s="17"/>
-      <c r="AG1" s="17"/>
-      <c r="AH1" s="17"/>
-      <c r="AI1" s="21"/>
+      <c r="AD1" s="16"/>
+      <c r="AE1" s="16"/>
+      <c r="AF1" s="16"/>
+      <c r="AG1" s="16"/>
+      <c r="AH1" s="16"/>
+      <c r="AI1" s="20"/>
       <c r="AJ1" s="2" t="s">
         <v>7</v>
       </c>
@@ -565,88 +556,88 @@
       <c r="G2" s="8">
         <v>31</v>
       </c>
-      <c r="H2" s="18">
+      <c r="H2" s="17">
         <v>1</v>
       </c>
-      <c r="I2" s="18">
+      <c r="I2" s="17">
         <v>2</v>
       </c>
-      <c r="J2" s="18">
+      <c r="J2" s="17">
         <v>3</v>
       </c>
-      <c r="K2" s="18">
+      <c r="K2" s="17">
         <v>4</v>
       </c>
-      <c r="L2" s="19">
+      <c r="L2" s="18">
         <v>5</v>
       </c>
-      <c r="M2" s="20">
+      <c r="M2" s="19">
         <v>6</v>
       </c>
-      <c r="N2" s="18">
+      <c r="N2" s="17">
         <v>7</v>
       </c>
-      <c r="O2" s="18">
+      <c r="O2" s="17">
         <v>8</v>
       </c>
-      <c r="P2" s="18">
+      <c r="P2" s="17">
         <v>9</v>
       </c>
-      <c r="Q2" s="18">
+      <c r="Q2" s="17">
         <v>10</v>
       </c>
-      <c r="R2" s="18">
+      <c r="R2" s="17">
         <v>11</v>
       </c>
-      <c r="S2" s="19">
-        <v>12</v>
-      </c>
-      <c r="T2" s="20">
+      <c r="S2" s="18">
+        <v>12</v>
+      </c>
+      <c r="T2" s="19">
         <v>13</v>
       </c>
-      <c r="U2" s="18">
+      <c r="U2" s="17">
         <v>14</v>
       </c>
-      <c r="V2" s="18">
+      <c r="V2" s="17">
         <v>15</v>
       </c>
-      <c r="W2" s="18">
+      <c r="W2" s="17">
         <v>16</v>
       </c>
-      <c r="X2" s="18">
-        <v>17</v>
-      </c>
-      <c r="Y2" s="18">
+      <c r="X2" s="17">
+        <v>17</v>
+      </c>
+      <c r="Y2" s="17">
         <v>18</v>
       </c>
-      <c r="Z2" s="19">
+      <c r="Z2" s="18">
         <v>19</v>
       </c>
-      <c r="AA2" s="20">
+      <c r="AA2" s="19">
         <v>20</v>
       </c>
-      <c r="AB2" s="18">
+      <c r="AB2" s="17">
         <v>21</v>
       </c>
-      <c r="AC2" s="18">
+      <c r="AC2" s="17">
         <v>22</v>
       </c>
-      <c r="AD2" s="18">
+      <c r="AD2" s="17">
         <v>23</v>
       </c>
-      <c r="AE2" s="18">
+      <c r="AE2" s="17">
         <v>24</v>
       </c>
-      <c r="AF2" s="18">
+      <c r="AF2" s="17">
         <v>25</v>
       </c>
-      <c r="AG2" s="19">
+      <c r="AG2" s="18">
         <v>26</v>
       </c>
-      <c r="AH2" s="20">
+      <c r="AH2" s="19">
         <v>27</v>
       </c>
-      <c r="AI2" s="18">
+      <c r="AI2" s="17">
         <v>28</v>
       </c>
       <c r="AJ2" s="11">
@@ -1919,7 +1910,7 @@
         <v>45</v>
       </c>
       <c r="B23" s="15"/>
-      <c r="C23" s="16" t="s">
+      <c r="C23" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -2091,9 +2082,7 @@
       <c r="A26" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="15" t="s">
-        <v>51</v>
-      </c>
+      <c r="B26" s="15"/>
       <c r="C26" s="1" t="s">
         <v>17</v>
       </c>
@@ -2148,7 +2137,7 @@
     </row>
     <row r="27" spans="1:37">
       <c r="A27" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B27" s="15"/>
       <c r="C27" s="1" t="s">
@@ -2205,9 +2194,11 @@
     </row>
     <row r="28" spans="1:37">
       <c r="A28" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="15"/>
       <c r="C28" s="1" t="s">
         <v>12</v>
       </c>

</xml_diff>